<commit_message>
fix price_after_discount and discount
</commit_message>
<xml_diff>
--- a/files/product-new-v1.xlsx
+++ b/files/product-new-v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmoud.maher\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\aghezty_v2_php7\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -44,9 +44,6 @@
     <t>discount</t>
   </si>
   <si>
-    <t>price_aftert_discount</t>
-  </si>
-  <si>
     <t>stock</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>brand</t>
+  </si>
+  <si>
+    <t>price_after_discount</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,10 +521,10 @@
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -545,45 +545,45 @@
         <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="M1" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
       </c>
       <c r="G2">
         <v>1000</v>
@@ -598,19 +598,19 @@
         <v>40</v>
       </c>
       <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
         <v>14</v>
       </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s">
         <v>23</v>
-      </c>
-      <c r="O2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add property to product excel
</commit_message>
<xml_diff>
--- a/files/product-new-v1.xlsx
+++ b/files/product-new-v1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>description_ar</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>price_after_discount</t>
+  </si>
+  <si>
+    <t>Flat, 45 Cm, Citrus Juicer, Electric Water Heater</t>
+  </si>
+  <si>
+    <t>property</t>
   </si>
 </sst>
 </file>
@@ -139,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +160,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -201,7 +213,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -212,6 +224,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -496,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,9 +532,10 @@
     <col min="13" max="13" width="24" customWidth="1"/>
     <col min="14" max="14" width="27.5703125" customWidth="1"/>
     <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -565,8 +581,11 @@
       <c r="O1" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="P1" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -611,6 +630,9 @@
       </c>
       <c r="O2" t="s">
         <v>23</v>
+      </c>
+      <c r="P2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add property to excel that used for create product
</commit_message>
<xml_diff>
--- a/files/product-new-v1.xlsx
+++ b/files/product-new-v1.xlsx
@@ -104,10 +104,10 @@
     <t>price_after_discount</t>
   </si>
   <si>
-    <t>Flat, 45 Cm, Citrus Juicer, Electric Water Heater</t>
-  </si>
-  <si>
     <t>property</t>
+  </si>
+  <si>
+    <t>Cooling Only,Air Curtains,1.5 HP</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +582,7 @@
         <v>24</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -632,7 +632,7 @@
         <v>23</v>
       </c>
       <c r="P2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
handle filter in excel in create product
</commit_message>
<xml_diff>
--- a/files/product-new-v1.xlsx
+++ b/files/product-new-v1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>description_ar</t>
   </si>
@@ -104,10 +104,25 @@
     <t>price_after_discount</t>
   </si>
   <si>
-    <t>property</t>
-  </si>
-  <si>
-    <t>Cooling Only,Air Curtains,1.5 HP</t>
+    <t>Cooling Only</t>
+  </si>
+  <si>
+    <t>Desert</t>
+  </si>
+  <si>
+    <t>6 HP</t>
+  </si>
+  <si>
+    <t>filter1</t>
+  </si>
+  <si>
+    <t>filter2</t>
+  </si>
+  <si>
+    <t>filter3</t>
+  </si>
+  <si>
+    <t>filter4</t>
   </si>
 </sst>
 </file>
@@ -511,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,10 +547,10 @@
     <col min="13" max="13" width="24" customWidth="1"/>
     <col min="14" max="14" width="27.5703125" customWidth="1"/>
     <col min="15" max="15" width="16.7109375" customWidth="1"/>
-    <col min="16" max="16" width="45.85546875" customWidth="1"/>
+    <col min="16" max="19" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -582,10 +597,19 @@
         <v>24</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -632,10 +656,24 @@
         <v>23</v>
       </c>
       <c r="P2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2">
+      <formula1>"Cooling Only,Desert,1.25 HP,6 HP"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2 Q2 R2">
+      <formula1>"Cooling Only,Desert,1.25 HP,6 HP"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>